<commit_message>
he incorporado la pasarela definitiva en las capas de usos del suelo
</commit_message>
<xml_diff>
--- a/Correspondencias_SIOSE - modificada (v5).xlsx
+++ b/Correspondencias_SIOSE - modificada (v5).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="179">
   <si>
     <t>SIOSE</t>
   </si>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t>Regadio</t>
+  </si>
+  <si>
+    <t>CAMPING</t>
   </si>
 </sst>
 </file>
@@ -717,21 +720,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color theme="0" tint="-0.249977111117893"/>
@@ -769,15 +757,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -790,16 +769,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -826,42 +830,51 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1145,17 +1158,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B68" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D113" sqref="B105:D113"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="70.85546875" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1"/>
@@ -1165,39 +1178,39 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>0</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>0</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1205,19 +1218,19 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>101</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>111</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>1</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1225,19 +1238,19 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>130</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>111</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>1</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1245,19 +1258,19 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>132</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>111</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>1</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1265,19 +1278,19 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>170</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>111</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>1</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1285,19 +1298,19 @@
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>171</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>111</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>1</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1305,59 +1318,59 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>2000</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>439</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>1</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>2002</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>115</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>1</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>117</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>117</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>2</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1365,19 +1378,19 @@
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>119</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>121</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>3</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1385,19 +1398,19 @@
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>120</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>121</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>3</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1405,19 +1418,19 @@
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>122</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>121</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>3</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1425,19 +1438,19 @@
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>125</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>111</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>3</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1445,19 +1458,19 @@
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>168</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>121</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>3</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1465,19 +1478,19 @@
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>131</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>131</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>4</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1485,19 +1498,19 @@
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>182</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>131</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="8">
         <v>4</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1505,39 +1518,39 @@
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>2004</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>131</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>4</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>154</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>141</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>5</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1545,19 +1558,19 @@
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>152</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>141</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>6</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1565,19 +1578,19 @@
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>162</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>141</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <v>6</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1585,99 +1598,99 @@
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>164</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>141</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="8">
         <v>6</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>113</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>141</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="8">
         <v>7</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <v>151</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>151</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>8</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <v>2007</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="12">
         <v>151</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="8">
         <v>9</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="9" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <v>153</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>153</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="8">
         <v>10</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1685,19 +1698,19 @@
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <v>106</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>193</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="8">
         <v>11</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1705,19 +1718,19 @@
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <v>123</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>191</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="8">
         <v>11</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1725,19 +1738,19 @@
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <v>136</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <v>193</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="8">
         <v>11</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1745,19 +1758,19 @@
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="6">
         <v>138</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>193</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="8">
         <v>11</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1765,19 +1778,19 @@
       <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="6">
         <v>142</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>193</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="8">
         <v>11</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1785,19 +1798,19 @@
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="6">
         <v>144</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="6">
         <v>193</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="8">
         <v>11</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1805,19 +1818,19 @@
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="6">
         <v>177</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="6">
         <v>191</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="8">
         <v>11</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1825,19 +1838,19 @@
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="6">
         <v>2005</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="6">
         <v>191</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="8">
         <v>11</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1845,19 +1858,19 @@
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <v>210</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="6">
         <v>211</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="8">
         <v>12</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1865,19 +1878,19 @@
       <c r="A36" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="6">
         <v>217</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <v>217</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="8">
         <v>12</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1885,19 +1898,19 @@
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="6">
         <v>2151</v>
       </c>
-      <c r="C37" s="13">
+      <c r="C37" s="12">
         <v>215</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="8">
         <v>12</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1905,99 +1918,99 @@
       <c r="A38" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="6">
         <v>2152</v>
       </c>
-      <c r="C38" s="13">
+      <c r="C38" s="12">
         <v>217</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="8">
         <v>12</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="6">
         <v>203</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="6">
         <v>225</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="8">
         <v>13</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F39" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="6">
         <v>221</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="6">
         <v>221</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40" s="8">
         <v>13</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="F40" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" s="6">
         <v>291</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="6">
         <v>291</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E41" s="8">
         <v>14</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F41" s="9" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="6">
         <v>960</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E42" s="8">
         <v>15</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="9" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2005,19 +2018,19 @@
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="6">
         <v>310</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E43" s="8">
         <v>16</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="9" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2025,199 +2038,199 @@
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="6">
         <v>318</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="6">
         <v>311</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E44" s="9">
+      <c r="E44" s="8">
         <v>16</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="9" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="6">
         <v>200</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="6">
         <v>331</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E45" s="9">
+      <c r="E45" s="8">
         <v>17</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F45" s="9" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="6">
         <v>315</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="6">
         <v>315</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E46" s="9">
+      <c r="E46" s="8">
         <v>17</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="9" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="6">
         <v>317</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="6">
         <v>317</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E47" s="8">
         <v>17</v>
       </c>
-      <c r="F47" s="10" t="s">
+      <c r="F47" s="9" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="6">
         <v>319</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="6">
         <v>321</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E48" s="9">
+      <c r="E48" s="8">
         <v>18</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="9" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="6">
         <v>2008</v>
       </c>
-      <c r="C49" s="13">
+      <c r="C49" s="12">
         <v>321</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E49" s="8">
         <v>19</v>
       </c>
-      <c r="F49" s="10" t="s">
+      <c r="F49" s="9" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B50" s="6">
         <v>332</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="6">
         <v>331</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E50" s="9">
+      <c r="E50" s="8">
         <v>20</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="F50" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="6">
         <v>341</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="6">
         <v>341</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E51" s="9">
+      <c r="E51" s="8">
         <v>21</v>
       </c>
-      <c r="F51" s="10" t="s">
+      <c r="F51" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="6">
         <v>345</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="6">
         <v>345</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E52" s="9">
+      <c r="E52" s="8">
         <v>22</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="6">
         <v>405</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E53" s="9">
+      <c r="E53" s="8">
         <v>23</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F53" s="9" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2225,19 +2238,19 @@
       <c r="A54" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B54" s="6">
         <v>416</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54" s="6">
         <v>415</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E54" s="9">
+      <c r="E54" s="8">
         <v>27</v>
       </c>
-      <c r="F54" s="10" t="s">
+      <c r="F54" s="9" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2245,19 +2258,19 @@
       <c r="A55" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="6">
         <v>460</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55" s="6">
         <v>419</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E55" s="8">
         <v>27</v>
       </c>
-      <c r="F55" s="10" t="s">
+      <c r="F55" s="9" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2265,19 +2278,19 @@
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="7">
+      <c r="B56" s="6">
         <v>403</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C56" s="6">
         <v>423</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E56" s="9">
+      <c r="E56" s="8">
         <v>26</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="F56" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2285,59 +2298,59 @@
       <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="7">
+      <c r="B57" s="6">
         <v>404</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="6">
         <v>423</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D57" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E57" s="9">
+      <c r="E57" s="8">
         <v>26</v>
       </c>
-      <c r="F57" s="10" t="s">
+      <c r="F57" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="7">
+      <c r="B58" s="6">
         <v>431</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C58" s="6">
         <v>431</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="D58" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E58" s="9">
+      <c r="E58" s="8">
         <v>28</v>
       </c>
-      <c r="F58" s="10" t="s">
+      <c r="F58" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B59" s="7">
+      <c r="B59" s="6">
         <v>997</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="6">
         <v>997</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="D59" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E59" s="9">
+      <c r="E59" s="8">
         <v>28</v>
       </c>
-      <c r="F59" s="10" t="s">
+      <c r="F59" s="9" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2345,359 +2358,359 @@
       <c r="A60" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" s="6">
         <v>4102</v>
       </c>
-      <c r="C60" s="13">
+      <c r="C60" s="12">
         <v>433</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="D60" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E60" s="9">
+      <c r="E60" s="8">
         <v>28</v>
       </c>
-      <c r="F60" s="10" t="s">
+      <c r="F60" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B61" s="7">
+      <c r="B61" s="6">
         <v>520</v>
       </c>
-      <c r="C61" s="7">
+      <c r="C61" s="6">
         <v>520</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D61" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="E61" s="9">
+      <c r="E61" s="8">
         <v>29</v>
       </c>
-      <c r="F61" s="10" t="s">
+      <c r="F61" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B62" s="7">
+      <c r="B62" s="6">
         <v>530</v>
       </c>
-      <c r="C62" s="7">
+      <c r="C62" s="6">
         <v>530</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="D62" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="E62" s="9">
+      <c r="E62" s="8">
         <v>29</v>
       </c>
-      <c r="F62" s="10" t="s">
+      <c r="F62" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B63" s="7">
+      <c r="B63" s="6">
         <v>621</v>
       </c>
-      <c r="C63" s="7">
+      <c r="C63" s="6">
         <v>621</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="D63" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="E63" s="9">
+      <c r="E63" s="8">
         <v>29</v>
       </c>
-      <c r="F63" s="10" t="s">
+      <c r="F63" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B64" s="7">
+      <c r="B64" s="6">
         <v>625</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C64" s="6">
         <v>625</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="D64" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E64" s="9">
+      <c r="E64" s="8">
         <v>29</v>
       </c>
-      <c r="F64" s="10" t="s">
+      <c r="F64" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="7">
+      <c r="B65" s="6">
         <v>721</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="6">
         <v>721</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="D65" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E65" s="9">
+      <c r="E65" s="8">
         <v>29</v>
       </c>
-      <c r="F65" s="10" t="s">
+      <c r="F65" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B66" s="7">
+      <c r="B66" s="6">
         <v>725</v>
       </c>
-      <c r="C66" s="7">
+      <c r="C66" s="6">
         <v>725</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="D66" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E66" s="9">
+      <c r="E66" s="8">
         <v>29</v>
       </c>
-      <c r="F66" s="10" t="s">
+      <c r="F66" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B67" s="7">
+      <c r="B67" s="6">
         <v>730</v>
       </c>
-      <c r="C67" s="7">
+      <c r="C67" s="6">
         <v>730</v>
       </c>
-      <c r="D67" s="8" t="s">
+      <c r="D67" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E67" s="9">
+      <c r="E67" s="8">
         <v>29</v>
       </c>
-      <c r="F67" s="10" t="s">
+      <c r="F67" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B68" s="7">
+      <c r="B68" s="6">
         <v>740</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C68" s="6">
         <v>740</v>
       </c>
-      <c r="D68" s="8" t="s">
+      <c r="D68" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E68" s="9">
+      <c r="E68" s="8">
         <v>29</v>
       </c>
-      <c r="F68" s="10" t="s">
+      <c r="F68" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B69" s="6">
         <v>821</v>
       </c>
-      <c r="C69" s="7">
+      <c r="C69" s="6">
         <v>821</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="D69" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E69" s="9">
+      <c r="E69" s="8">
         <v>29</v>
       </c>
-      <c r="F69" s="10" t="s">
+      <c r="F69" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B70" s="7">
+      <c r="B70" s="6">
         <v>825</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C70" s="6">
         <v>825</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D70" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E70" s="9">
+      <c r="E70" s="8">
         <v>29</v>
       </c>
-      <c r="F70" s="10" t="s">
+      <c r="F70" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B71" s="7">
+      <c r="B71" s="6">
         <v>830</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="6">
         <v>830</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="D71" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E71" s="9">
+      <c r="E71" s="8">
         <v>29</v>
       </c>
-      <c r="F71" s="10" t="s">
+      <c r="F71" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B72" s="7">
+      <c r="B72" s="6">
         <v>840</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72" s="6">
         <v>840</v>
       </c>
-      <c r="D72" s="8" t="s">
+      <c r="D72" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E72" s="9">
+      <c r="E72" s="8">
         <v>29</v>
       </c>
-      <c r="F72" s="10" t="s">
+      <c r="F72" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
+      <c r="A73" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B73" s="7">
+      <c r="B73" s="6">
         <v>911</v>
       </c>
-      <c r="C73" s="7">
+      <c r="C73" s="6">
         <v>911</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="D73" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E73" s="9">
+      <c r="E73" s="8">
         <v>30</v>
       </c>
-      <c r="F73" s="10" t="s">
+      <c r="F73" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B74" s="7">
+      <c r="B74" s="6">
         <v>915</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C74" s="6">
         <v>915</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="D74" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E74" s="9">
+      <c r="E74" s="8">
         <v>30</v>
       </c>
-      <c r="F74" s="10" t="s">
+      <c r="F74" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B75" s="7">
+      <c r="B75" s="6">
         <v>917</v>
       </c>
-      <c r="C75" s="7">
+      <c r="C75" s="6">
         <v>917</v>
       </c>
-      <c r="D75" s="8" t="s">
+      <c r="D75" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E75" s="9">
+      <c r="E75" s="8">
         <v>30</v>
       </c>
-      <c r="F75" s="10" t="s">
+      <c r="F75" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
+      <c r="A76" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B76" s="7">
+      <c r="B76" s="6">
         <v>921</v>
       </c>
-      <c r="C76" s="7">
+      <c r="C76" s="6">
         <v>921</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="D76" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E76" s="9">
+      <c r="E76" s="8">
         <v>31</v>
       </c>
-      <c r="F76" s="10" t="s">
+      <c r="F76" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
+      <c r="A77" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B77" s="6">
         <v>925</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C77" s="6">
         <v>925</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="D77" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E77" s="9">
+      <c r="E77" s="8">
         <v>31</v>
       </c>
-      <c r="F77" s="10" t="s">
+      <c r="F77" s="9" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2705,19 +2718,19 @@
       <c r="A78" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B78" s="7">
+      <c r="B78" s="6">
         <v>944</v>
       </c>
-      <c r="C78" s="7">
+      <c r="C78" s="6">
         <v>944</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="D78" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E78" s="9">
+      <c r="E78" s="8">
         <v>32</v>
       </c>
-      <c r="F78" s="10" t="s">
+      <c r="F78" s="9" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2725,19 +2738,19 @@
       <c r="A79" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B79" s="7">
+      <c r="B79" s="6">
         <v>9311</v>
       </c>
-      <c r="C79" s="13">
+      <c r="C79" s="12">
         <v>931</v>
       </c>
-      <c r="D79" s="8" t="s">
+      <c r="D79" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E79" s="9">
+      <c r="E79" s="8">
         <v>32</v>
       </c>
-      <c r="F79" s="10" t="s">
+      <c r="F79" s="9" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2745,400 +2758,420 @@
       <c r="A80" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B80" s="7">
+      <c r="B80" s="6">
         <v>9312</v>
       </c>
-      <c r="C80" s="13">
+      <c r="C80" s="12">
         <v>931</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D80" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E80" s="9">
+      <c r="E80" s="8">
         <v>32</v>
       </c>
-      <c r="F80" s="10" t="s">
+      <c r="F80" s="9" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
+      <c r="A81" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B81" s="7">
+      <c r="B81" s="6">
         <v>945</v>
       </c>
-      <c r="C81" s="7">
+      <c r="C81" s="6">
         <v>932</v>
       </c>
-      <c r="D81" s="8" t="s">
+      <c r="D81" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E81" s="9">
+      <c r="E81" s="8">
         <v>33</v>
       </c>
-      <c r="F81" s="10" t="s">
+      <c r="F81" s="9" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
+      <c r="A82" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B82" s="7">
+      <c r="B82" s="6">
         <v>933</v>
       </c>
-      <c r="C82" s="13">
+      <c r="C82" s="12">
         <v>933</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="D82" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E82" s="9">
+      <c r="E82" s="8">
         <v>34</v>
       </c>
-      <c r="F82" s="10" t="s">
+      <c r="F82" s="9" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="6" t="s">
+      <c r="A83" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B83" s="7">
+      <c r="B83" s="6">
         <v>935</v>
       </c>
-      <c r="C83" s="7">
+      <c r="C83" s="6">
         <v>935</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="D83" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E83" s="16">
+      <c r="E83" s="14">
         <v>35</v>
       </c>
-      <c r="F83" s="10" t="s">
+      <c r="F83" s="9" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="18" t="s">
+      <c r="A84" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B84" s="19" t="s">
+      <c r="B84" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C84" s="20">
+      <c r="C84" s="18">
         <v>155</v>
       </c>
-      <c r="D84" s="22" t="s">
+      <c r="D84" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="E84" s="17">
+      <c r="E84" s="15">
         <v>36</v>
       </c>
-      <c r="F84" s="14" t="s">
+      <c r="F84" s="13" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="18" t="s">
+      <c r="A85" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="B85" s="19" t="s">
+      <c r="B85" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C85" s="20">
+      <c r="C85" s="18">
         <v>231</v>
       </c>
-      <c r="D85" s="18" t="s">
+      <c r="D85" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="E85" s="17">
+      <c r="E85" s="15">
         <v>20</v>
       </c>
-      <c r="F85" s="10" t="s">
+      <c r="F85" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="21" t="s">
+      <c r="A86" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="B86" s="19" t="s">
+      <c r="B86" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C86" s="20">
+      <c r="C86" s="18">
         <v>411</v>
       </c>
-      <c r="D86" s="21" t="s">
+      <c r="D86" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="E86" s="17">
+      <c r="E86" s="15">
         <v>24</v>
       </c>
-      <c r="F86" s="14" t="s">
+      <c r="F86" s="13" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="15" t="s">
+      <c r="A87" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="B87" s="19" t="s">
+      <c r="B87" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="C87" s="13">
+      <c r="C87" s="12">
         <v>425</v>
       </c>
-      <c r="D87" s="15" t="s">
+      <c r="D87" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="E87" s="17">
+      <c r="E87" s="15">
         <v>25</v>
       </c>
-      <c r="F87" s="14" t="s">
+      <c r="F87" s="13" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="A88" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B88" s="19" t="s">
+      <c r="B88" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C88" s="23">
+      <c r="C88" s="18">
         <v>427</v>
       </c>
-      <c r="D88" s="24" t="s">
+      <c r="D88" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="E88" s="25">
+      <c r="E88" s="21">
         <v>25</v>
       </c>
-      <c r="F88" s="26" t="s">
+      <c r="F88" s="22" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="A89" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="B89" s="19" t="s">
+      <c r="B89" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C89" s="23">
+      <c r="C89" s="18">
         <v>441</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="E89" s="25">
+      <c r="E89" s="21">
         <v>27</v>
       </c>
-      <c r="F89" s="29" t="s">
+      <c r="F89" s="24" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="A90" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="B90" s="19" t="s">
+      <c r="B90" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="23">
+      <c r="C90" s="18">
         <v>451</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E90" s="25">
+      <c r="E90" s="21">
         <v>28</v>
       </c>
-      <c r="F90" s="29" t="s">
+      <c r="F90" s="24" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="A91" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="B91" s="19" t="s">
+      <c r="B91" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C91" s="23">
+      <c r="C91" s="18">
         <v>461</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E91" s="17">
+      <c r="E91" s="15">
         <v>25</v>
       </c>
-      <c r="F91" s="14" t="s">
+      <c r="F91" s="13" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="A92" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="B92" s="19" t="s">
+      <c r="B92" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C92" s="23">
+      <c r="C92" s="18">
         <v>471</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E92" s="25">
+      <c r="E92" s="21">
         <v>37</v>
       </c>
-      <c r="F92" s="28" t="s">
+      <c r="F92" s="23" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="A93" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="B93" s="19" t="s">
+      <c r="B93" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C93" s="23">
+      <c r="C93" s="18">
         <v>473</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="E93" s="27">
+      <c r="E93" s="25">
         <v>37</v>
       </c>
-      <c r="F93" s="28" t="s">
+      <c r="F93" s="23" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="A94" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="B94" s="19" t="s">
+      <c r="B94" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C94" s="23">
+      <c r="C94" s="18">
         <v>475</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="E94" s="25">
+      <c r="E94" s="21">
         <v>37</v>
       </c>
-      <c r="F94" s="28" t="s">
+      <c r="F94" s="23" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="A95" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="B95" s="19" t="s">
+      <c r="B95" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C95" s="23">
+      <c r="C95" s="18">
         <v>477</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="E95" s="25">
+      <c r="E95" s="21">
         <v>37</v>
       </c>
-      <c r="F95" s="28" t="s">
+      <c r="F95" s="23" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="A96" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="B96" s="19" t="s">
+      <c r="B96" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C96" s="23">
+      <c r="C96" s="18">
         <v>479</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E96" s="25">
+      <c r="E96" s="21">
         <v>37</v>
       </c>
-      <c r="F96" s="28" t="s">
+      <c r="F96" s="23" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="A97" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="B97" s="19" t="s">
+      <c r="B97" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C97" s="23">
+      <c r="C97" s="18">
         <v>570</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E97" s="9">
+      <c r="E97" s="14">
         <v>29</v>
       </c>
-      <c r="F97" s="10" t="s">
+      <c r="F97" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="A98" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="B98" s="19" t="s">
+      <c r="B98" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C98" s="23">
+      <c r="C98" s="18">
         <v>611</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="E98" s="9">
+      <c r="E98" s="14">
         <v>29</v>
       </c>
-      <c r="F98" s="10" t="s">
+      <c r="F98" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="A99" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="B99" s="19" t="s">
+      <c r="B99" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C99" s="23">
+      <c r="C99" s="18">
         <v>465</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="E99" s="27">
+      <c r="E99" s="25">
         <v>37</v>
       </c>
-      <c r="F99" s="28" t="s">
+      <c r="F99" s="23" t="s">
         <v>175</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B100" s="29">
+        <v>172</v>
+      </c>
+      <c r="C100" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="D100" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E100" s="8">
+        <v>11</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
he corregido errores que habia en las capas del proyecto y he reunido las capas de usos con la pasarela actualizada
</commit_message>
<xml_diff>
--- a/Correspondencias_SIOSE - modificada (v5).xlsx
+++ b/Correspondencias_SIOSE - modificada (v5).xlsx
@@ -3104,7 +3104,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
@@ -3177,33 +3177,28 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -3497,9 +3492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3543,2430 +3536,2432 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
       <c r="C2" s="6">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="D2" s="6">
-        <v>141</v>
+        <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="8"/>
+        <v>5</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
       <c r="G2" s="9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>52</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>59</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C3" s="6">
-        <v>405</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>60</v>
+        <v>101</v>
+      </c>
+      <c r="D3" s="6">
+        <v>111</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="F3" s="8">
-        <v>14</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="C4" s="6">
-        <v>416</v>
+        <v>130</v>
       </c>
       <c r="D4" s="6">
-        <v>415</v>
+        <v>111</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="F4" s="8">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6">
-        <v>460</v>
+        <v>132</v>
       </c>
       <c r="D5" s="6">
-        <v>419</v>
+        <v>111</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>118</v>
+        <v>24</v>
       </c>
       <c r="F5" s="8">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="C6" s="6">
-        <v>403</v>
+        <v>170</v>
       </c>
       <c r="D6" s="6">
-        <v>423</v>
+        <v>111</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="F6" s="8">
-        <v>17</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>923</v>
+        <v>1</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="C7" s="6">
-        <v>404</v>
+        <v>171</v>
       </c>
       <c r="D7" s="6">
-        <v>423</v>
+        <v>111</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="F7" s="8">
-        <v>17</v>
-      </c>
-      <c r="G7" s="28" t="s">
-        <v>923</v>
+        <v>1</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I7">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>57</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>64</v>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C8" s="6">
-        <v>431</v>
+        <v>2000</v>
       </c>
       <c r="D8" s="6">
-        <v>431</v>
+        <v>439</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="F8" s="8">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I8">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C9" s="6">
-        <v>997</v>
+        <v>2002</v>
       </c>
       <c r="D9" s="6">
-        <v>997</v>
+        <v>115</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F9" s="8">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I9">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>59</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>129</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="C10" s="6">
-        <v>4102</v>
-      </c>
-      <c r="D10" s="11">
-        <v>433</v>
+        <v>117</v>
+      </c>
+      <c r="D10" s="6">
+        <v>117</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="F10" s="8">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I10">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>85</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D11" s="11">
-        <v>411</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>152</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="6">
+        <v>119</v>
+      </c>
+      <c r="D11" s="6">
+        <v>121</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="F11" s="8">
-        <v>18</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>924</v>
+        <v>2</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I11">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>86</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D12" s="11">
-        <v>425</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>153</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="6">
+        <v>120</v>
+      </c>
+      <c r="D12" s="6">
+        <v>121</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>122</v>
       </c>
       <c r="F12" s="8">
-        <v>18</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>924</v>
+        <v>2</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>87</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D13" s="11">
-        <v>427</v>
-      </c>
-      <c r="E13" s="44" t="s">
-        <v>154</v>
-      </c>
-      <c r="F13" s="45">
-        <v>18</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>924</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="6">
+        <v>122</v>
+      </c>
+      <c r="D13" s="6">
+        <v>121</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="8">
+        <v>2</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I13">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>88</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D14" s="11">
-        <v>441</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="F14" s="45">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="6">
+        <v>125</v>
+      </c>
+      <c r="D14" s="6">
+        <v>111</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="17" t="s">
-        <v>168</v>
+      <c r="F14" s="8">
+        <v>2</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I14">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>89</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D15" s="11">
-        <v>451</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="F15" s="45">
-        <v>19</v>
-      </c>
-      <c r="G15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="6">
         <v>168</v>
       </c>
+      <c r="D15" s="6">
+        <v>121</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="8">
+        <v>2</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="H15" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I15">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>90</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D16" s="11">
-        <v>461</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>156</v>
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="6">
+        <v>131</v>
+      </c>
+      <c r="D16" s="6">
+        <v>131</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="F16" s="8">
-        <v>18</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>924</v>
+        <v>3</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="H16" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I16">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>91</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D17" s="11">
-        <v>471</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="F17" s="45">
-        <v>19</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>168</v>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="6">
+        <v>182</v>
+      </c>
+      <c r="D17" s="6">
+        <v>131</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="8">
+        <v>3</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="H17" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I17">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>92</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D18" s="11">
-        <v>473</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="F18" s="45">
-        <v>19</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>168</v>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="6">
+        <v>2004</v>
+      </c>
+      <c r="D18" s="6">
+        <v>131</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="8">
+        <v>3</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="H18" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I18">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>93</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="C19" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="11">
-        <v>475</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="F19" s="45">
-        <v>19</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>168</v>
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="6">
+        <v>154</v>
+      </c>
+      <c r="D19" s="6">
+        <v>141</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="8">
+        <v>4</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="H19" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I19">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>94</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D20" s="11">
-        <v>477</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="F20" s="45">
         <v>19</v>
       </c>
-      <c r="G20" s="17" t="s">
-        <v>168</v>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="6">
+        <v>152</v>
+      </c>
+      <c r="D20" s="6">
+        <v>141</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="8">
+        <v>4</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="H20" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I20">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>95</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>158</v>
-      </c>
-      <c r="C21" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D21" s="11">
-        <v>479</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>158</v>
-      </c>
-      <c r="F21" s="45">
-        <v>19</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>168</v>
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="6">
+        <v>162</v>
+      </c>
+      <c r="D21" s="6">
+        <v>141</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="8">
+        <v>4</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="H21" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I21">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>98</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D22" s="11">
-        <v>465</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="F22" s="45">
-        <v>19</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>168</v>
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="6">
+        <v>164</v>
+      </c>
+      <c r="D22" s="6">
+        <v>141</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="8">
+        <v>4</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="H22" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I22">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="C23" s="6">
-        <v>520</v>
+        <v>113</v>
       </c>
       <c r="D23" s="6">
-        <v>520</v>
+        <v>141</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>147</v>
+        <v>12</v>
       </c>
       <c r="F23" s="8">
-        <v>20</v>
-      </c>
-      <c r="G23" s="29" t="s">
-        <v>920</v>
+        <v>19</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="H23" t="s">
-        <v>932</v>
+        <v>927</v>
       </c>
       <c r="I23">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="C24" s="6">
-        <v>530</v>
+        <v>151</v>
       </c>
       <c r="D24" s="6">
-        <v>530</v>
+        <v>151</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="F24" s="8">
-        <v>21</v>
-      </c>
-      <c r="G24" s="29" t="s">
-        <v>921</v>
+        <v>5</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>918</v>
       </c>
       <c r="H24" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="I24">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="C25" s="6">
-        <v>621</v>
-      </c>
-      <c r="D25" s="6">
-        <v>621</v>
+        <v>2007</v>
+      </c>
+      <c r="D25" s="11">
+        <v>151</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="F25" s="8">
-        <v>20</v>
-      </c>
-      <c r="G25" s="29" t="s">
-        <v>920</v>
+        <v>5</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>918</v>
       </c>
       <c r="H25" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="I25">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="C26" s="6">
-        <v>625</v>
+        <v>153</v>
       </c>
       <c r="D26" s="6">
-        <v>625</v>
+        <v>153</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>131</v>
+        <v>33</v>
       </c>
       <c r="F26" s="8">
-        <v>20</v>
-      </c>
-      <c r="G26" s="29" t="s">
-        <v>920</v>
+        <v>5</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>918</v>
       </c>
       <c r="H26" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="I26">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>64</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>71</v>
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C27" s="6">
-        <v>721</v>
+        <v>106</v>
       </c>
       <c r="D27" s="6">
-        <v>721</v>
+        <v>193</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="F27" s="8">
-        <v>20</v>
-      </c>
-      <c r="G27" s="29" t="s">
-        <v>920</v>
+        <v>6</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="H27" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="I27">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>65</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>72</v>
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C28" s="6">
-        <v>725</v>
+        <v>123</v>
       </c>
       <c r="D28" s="6">
-        <v>725</v>
+        <v>191</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>133</v>
+        <v>18</v>
       </c>
       <c r="F28" s="8">
-        <v>20</v>
-      </c>
-      <c r="G28" s="29" t="s">
-        <v>920</v>
+        <v>6</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="H28" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="I28">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>66</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>73</v>
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C29" s="6">
-        <v>730</v>
+        <v>136</v>
       </c>
       <c r="D29" s="6">
-        <v>730</v>
+        <v>193</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="F29" s="8">
-        <v>21</v>
-      </c>
-      <c r="G29" s="29" t="s">
-        <v>921</v>
+        <v>6</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="H29" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="I29">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>67</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>75</v>
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C30" s="6">
-        <v>740</v>
+        <v>138</v>
       </c>
       <c r="D30" s="6">
-        <v>740</v>
+        <v>193</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="F30" s="8">
-        <v>20</v>
-      </c>
-      <c r="G30" s="29" t="s">
-        <v>920</v>
+        <v>6</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="I30">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>68</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>77</v>
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C31" s="6">
-        <v>821</v>
+        <v>142</v>
       </c>
       <c r="D31" s="6">
-        <v>821</v>
+        <v>193</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>134</v>
+        <v>26</v>
       </c>
       <c r="F31" s="8">
-        <v>20</v>
-      </c>
-      <c r="G31" s="29" t="s">
-        <v>920</v>
+        <v>6</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="H31" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="I31">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>69</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>78</v>
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C32" s="6">
-        <v>825</v>
+        <v>144</v>
       </c>
       <c r="D32" s="6">
-        <v>825</v>
+        <v>193</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>135</v>
+        <v>27</v>
       </c>
       <c r="F32" s="8">
-        <v>20</v>
-      </c>
-      <c r="G32" s="29" t="s">
-        <v>920</v>
+        <v>6</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="H32" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="I32">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>70</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>79</v>
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C33" s="6">
-        <v>830</v>
+        <v>177</v>
       </c>
       <c r="D33" s="6">
-        <v>830</v>
+        <v>191</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>80</v>
+        <v>124</v>
       </c>
       <c r="F33" s="8">
-        <v>21</v>
-      </c>
-      <c r="G33" s="29" t="s">
-        <v>921</v>
+        <v>6</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="H33" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="I33">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>71</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>81</v>
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C34" s="6">
-        <v>840</v>
+        <v>2005</v>
       </c>
       <c r="D34" s="6">
-        <v>840</v>
+        <v>191</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="F34" s="8">
-        <v>20</v>
-      </c>
-      <c r="G34" s="29" t="s">
-        <v>920</v>
+        <v>6</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="H34" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="I34">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>72</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>83</v>
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C35" s="6">
-        <v>911</v>
+        <v>210</v>
       </c>
       <c r="D35" s="6">
-        <v>911</v>
+        <v>211</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>84</v>
+        <v>140</v>
       </c>
       <c r="F35" s="8">
-        <v>20</v>
-      </c>
-      <c r="G35" s="29" t="s">
-        <v>920</v>
+        <v>7</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="H35" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I35">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>73</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>85</v>
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="C36" s="6">
-        <v>915</v>
+        <v>217</v>
       </c>
       <c r="D36" s="6">
-        <v>915</v>
+        <v>217</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>86</v>
+        <v>141</v>
       </c>
       <c r="F36" s="8">
-        <v>20</v>
-      </c>
-      <c r="G36" s="29" t="s">
-        <v>920</v>
+        <v>7</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="H36" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I36">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>74</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>87</v>
+        <v>36</v>
+      </c>
+      <c r="B37" s="31" t="s">
+        <v>42</v>
       </c>
       <c r="C37" s="6">
-        <v>917</v>
-      </c>
-      <c r="D37" s="6">
-        <v>917</v>
+        <v>2151</v>
+      </c>
+      <c r="D37" s="11">
+        <v>215</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
       <c r="F37" s="8">
-        <v>20</v>
-      </c>
-      <c r="G37" s="29" t="s">
-        <v>920</v>
+        <v>7</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="H37" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I37">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>75</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>89</v>
+        <v>37</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>45</v>
       </c>
       <c r="C38" s="6">
-        <v>921</v>
-      </c>
-      <c r="D38" s="6">
-        <v>921</v>
+        <v>2152</v>
+      </c>
+      <c r="D38" s="11">
+        <v>217</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>90</v>
+        <v>143</v>
       </c>
       <c r="F38" s="8">
-        <v>20</v>
-      </c>
-      <c r="G38" s="29" t="s">
-        <v>920</v>
+        <v>7</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="H38" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I38">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>76</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>91</v>
+        <v>38</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>39</v>
       </c>
       <c r="C39" s="6">
-        <v>925</v>
+        <v>203</v>
       </c>
       <c r="D39" s="6">
-        <v>925</v>
+        <v>225</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="F39" s="8">
-        <v>20</v>
-      </c>
-      <c r="G39" s="29" t="s">
-        <v>920</v>
+        <v>8</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="H39" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I39">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>77</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>97</v>
+        <v>39</v>
+      </c>
+      <c r="B40" s="32" t="s">
+        <v>39</v>
       </c>
       <c r="C40" s="6">
-        <v>944</v>
+        <v>221</v>
       </c>
       <c r="D40" s="6">
-        <v>944</v>
+        <v>221</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="F40" s="8">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="H40" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I40">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>78</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>97</v>
+        <v>40</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>47</v>
       </c>
       <c r="C41" s="6">
-        <v>9311</v>
-      </c>
-      <c r="D41" s="11">
-        <v>931</v>
+        <v>291</v>
+      </c>
+      <c r="D41" s="6">
+        <v>291</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="F41" s="8">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="H41" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I41">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>79</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>97</v>
+        <v>41</v>
+      </c>
+      <c r="B42" s="32" t="s">
+        <v>102</v>
       </c>
       <c r="C42" s="6">
-        <v>9312</v>
-      </c>
-      <c r="D42" s="11">
-        <v>931</v>
+        <v>960</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F42" s="8">
-        <v>22</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>99</v>
+        <v>10</v>
+      </c>
+      <c r="G42" s="29" t="s">
+        <v>919</v>
       </c>
       <c r="H42" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I42">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>80</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>100</v>
+        <v>42</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>48</v>
       </c>
       <c r="C43" s="6">
-        <v>945</v>
-      </c>
-      <c r="D43" s="6">
-        <v>932</v>
+        <v>310</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="F43" s="8">
-        <v>23</v>
-      </c>
-      <c r="G43" s="27" t="s">
-        <v>94</v>
+        <v>10</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>919</v>
       </c>
       <c r="H43" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I43">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>81</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>93</v>
+        <v>43</v>
+      </c>
+      <c r="B44" s="31" t="s">
+        <v>48</v>
       </c>
       <c r="C44" s="6">
-        <v>933</v>
-      </c>
-      <c r="D44" s="11">
-        <v>933</v>
+        <v>318</v>
+      </c>
+      <c r="D44" s="6">
+        <v>311</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F44" s="8">
-        <v>23</v>
-      </c>
-      <c r="G44" s="27" t="s">
-        <v>94</v>
+        <v>10</v>
+      </c>
+      <c r="G44" s="29" t="s">
+        <v>919</v>
       </c>
       <c r="H44" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I44">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>82</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>95</v>
+        <v>44</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>38</v>
       </c>
       <c r="C45" s="6">
-        <v>935</v>
+        <v>200</v>
       </c>
       <c r="D45" s="6">
-        <v>935</v>
+        <v>331</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>96</v>
+        <v>145</v>
       </c>
       <c r="F45" s="8">
-        <v>23</v>
-      </c>
-      <c r="G45" s="27" t="s">
-        <v>94</v>
+        <v>11</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="H45" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I45">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>96</v>
-      </c>
-      <c r="B46" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="C46" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D46" s="11">
-        <v>570</v>
-      </c>
-      <c r="E46" s="32" t="s">
-        <v>159</v>
+        <v>45</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="6">
+        <v>315</v>
+      </c>
+      <c r="D46" s="6">
+        <v>315</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="F46" s="8">
-        <v>21</v>
-      </c>
-      <c r="G46" s="29" t="s">
-        <v>921</v>
+        <v>11</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="H46" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I46">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>97</v>
-      </c>
-      <c r="B47" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="C47" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D47" s="11">
-        <v>611</v>
-      </c>
-      <c r="E47" s="32" t="s">
-        <v>160</v>
+        <v>46</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="6">
+        <v>317</v>
+      </c>
+      <c r="D47" s="6">
+        <v>317</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="F47" s="8">
-        <v>20</v>
-      </c>
-      <c r="G47" s="29" t="s">
-        <v>920</v>
+        <v>11</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="H47" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I47">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>23</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>28</v>
+        <v>47</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>49</v>
       </c>
       <c r="C48" s="6">
-        <v>151</v>
+        <v>319</v>
       </c>
       <c r="D48" s="6">
-        <v>151</v>
+        <v>321</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="F48" s="8">
-        <v>5</v>
-      </c>
-      <c r="G48" s="28" t="s">
-        <v>918</v>
+        <v>10</v>
+      </c>
+      <c r="G48" s="29" t="s">
+        <v>919</v>
       </c>
       <c r="H48" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="I48">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>24</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>28</v>
+        <v>48</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>49</v>
       </c>
       <c r="C49" s="6">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="D49" s="11">
-        <v>151</v>
+        <v>321</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F49" s="8">
-        <v>5</v>
-      </c>
-      <c r="G49" s="28" t="s">
-        <v>918</v>
+        <v>10</v>
+      </c>
+      <c r="G49" s="29" t="s">
+        <v>919</v>
       </c>
       <c r="H49" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="I49">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>25</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>32</v>
+        <v>49</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>50</v>
       </c>
       <c r="C50" s="6">
-        <v>153</v>
+        <v>332</v>
       </c>
       <c r="D50" s="6">
-        <v>153</v>
+        <v>331</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="F50" s="8">
-        <v>5</v>
-      </c>
-      <c r="G50" s="28" t="s">
-        <v>918</v>
+        <v>12</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="H50" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="I50">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>1</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>136</v>
+        <v>50</v>
+      </c>
+      <c r="B51" s="32" t="s">
+        <v>52</v>
       </c>
       <c r="C51" s="6">
-        <v>0</v>
+        <v>341</v>
       </c>
       <c r="D51" s="6">
-        <v>0</v>
+        <v>341</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="F51" s="8">
-        <v>0</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="G51" s="29" t="s">
+        <v>922</v>
       </c>
       <c r="H51" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="I51">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>2</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>6</v>
+        <v>51</v>
+      </c>
+      <c r="B52" s="32" t="s">
+        <v>54</v>
       </c>
       <c r="C52" s="6">
-        <v>101</v>
+        <v>345</v>
       </c>
       <c r="D52" s="6">
-        <v>111</v>
+        <v>345</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="F52" s="8">
-        <v>1</v>
-      </c>
-      <c r="G52" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="G52" s="29" t="s">
+        <v>922</v>
       </c>
       <c r="H52" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="I52">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>3</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>6</v>
+        <v>52</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="C53" s="6">
-        <v>130</v>
-      </c>
-      <c r="D53" s="6">
-        <v>111</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>20</v>
+        <v>405</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="F53" s="8">
-        <v>1</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="G53" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="H53" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I53">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="6">
+        <v>416</v>
+      </c>
+      <c r="D54" s="6">
+        <v>415</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F54" s="8">
+        <v>14</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H54" t="s">
+        <v>927</v>
+      </c>
+      <c r="I54">
         <v>4</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54" s="6">
-        <v>132</v>
-      </c>
-      <c r="D54" s="6">
-        <v>111</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F54" s="8">
-        <v>1</v>
-      </c>
-      <c r="G54" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H54" t="s">
-        <v>926</v>
-      </c>
-      <c r="I54">
-        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="C55" s="6">
-        <v>170</v>
+        <v>460</v>
       </c>
       <c r="D55" s="6">
-        <v>111</v>
+        <v>419</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="F55" s="8">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="H55" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I55">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C56" s="6">
-        <v>171</v>
+        <v>403</v>
       </c>
       <c r="D56" s="6">
-        <v>111</v>
+        <v>423</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="F56" s="8">
-        <v>1</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="G56" s="28" t="s">
+        <v>923</v>
       </c>
       <c r="H56" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I56">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C57" s="6">
-        <v>2000</v>
+        <v>404</v>
       </c>
       <c r="D57" s="6">
-        <v>439</v>
+        <v>423</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
       <c r="F57" s="8">
-        <v>1</v>
-      </c>
-      <c r="G57" s="9" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="G57" s="28" t="s">
+        <v>923</v>
       </c>
       <c r="H57" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="C58" s="6">
-        <v>2002</v>
+        <v>431</v>
       </c>
       <c r="D58" s="6">
-        <v>115</v>
+        <v>431</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="F58" s="8">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="H58" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I58">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="C59" s="6">
-        <v>117</v>
+        <v>997</v>
       </c>
       <c r="D59" s="6">
-        <v>117</v>
+        <v>997</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="F59" s="8">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="H59" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I59">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C60" s="6">
+        <v>4102</v>
+      </c>
+      <c r="D60" s="11">
+        <v>433</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F60" s="8">
         <v>15</v>
       </c>
-      <c r="C60" s="6">
-        <v>119</v>
-      </c>
-      <c r="D60" s="6">
-        <v>121</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F60" s="8">
-        <v>2</v>
-      </c>
       <c r="G60" s="9" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="H60" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I60">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>11</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>15</v>
+        <v>60</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="C61" s="6">
-        <v>120</v>
+        <v>520</v>
       </c>
       <c r="D61" s="6">
-        <v>121</v>
+        <v>520</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="F61" s="8">
-        <v>2</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="G61" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H61" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I61">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>12</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>15</v>
+        <v>61</v>
+      </c>
+      <c r="B62" s="32" t="s">
+        <v>68</v>
       </c>
       <c r="C62" s="6">
-        <v>122</v>
+        <v>530</v>
       </c>
       <c r="D62" s="6">
-        <v>121</v>
+        <v>530</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>17</v>
+        <v>148</v>
       </c>
       <c r="F62" s="8">
-        <v>2</v>
-      </c>
-      <c r="G62" s="9" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="G62" s="29" t="s">
+        <v>921</v>
       </c>
       <c r="H62" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I62">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>13</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>15</v>
+        <v>62</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="C63" s="6">
-        <v>125</v>
+        <v>621</v>
       </c>
       <c r="D63" s="6">
-        <v>111</v>
+        <v>621</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>19</v>
+        <v>130</v>
       </c>
       <c r="F63" s="8">
-        <v>2</v>
-      </c>
-      <c r="G63" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="G63" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H63" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I63">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>14</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>15</v>
+        <v>63</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C64" s="6">
-        <v>168</v>
+        <v>625</v>
       </c>
       <c r="D64" s="6">
-        <v>121</v>
+        <v>625</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="F64" s="8">
-        <v>2</v>
-      </c>
-      <c r="G64" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="G64" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H64" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I64">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>15</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>21</v>
+        <v>64</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="C65" s="6">
-        <v>131</v>
+        <v>721</v>
       </c>
       <c r="D65" s="6">
-        <v>131</v>
+        <v>721</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="F65" s="8">
-        <v>3</v>
-      </c>
-      <c r="G65" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="G65" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H65" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I65">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>16</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>21</v>
+        <v>65</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="C66" s="6">
-        <v>182</v>
+        <v>725</v>
       </c>
       <c r="D66" s="6">
-        <v>131</v>
+        <v>725</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F66" s="8">
-        <v>3</v>
-      </c>
-      <c r="G66" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="G66" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H66" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I66">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>17</v>
-      </c>
-      <c r="B67" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="6">
+        <v>730</v>
+      </c>
+      <c r="D67" s="6">
+        <v>730</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F67" s="8">
         <v>21</v>
       </c>
-      <c r="C67" s="6">
-        <v>2004</v>
-      </c>
-      <c r="D67" s="6">
-        <v>131</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="F67" s="8">
-        <v>3</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>23</v>
+      <c r="G67" s="29" t="s">
+        <v>921</v>
       </c>
       <c r="H67" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I67">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="C68" s="6">
-        <v>154</v>
+        <v>740</v>
       </c>
       <c r="D68" s="6">
-        <v>141</v>
+        <v>740</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>139</v>
+        <v>76</v>
       </c>
       <c r="F68" s="8">
-        <v>4</v>
-      </c>
-      <c r="G68" s="27" t="s">
-        <v>31</v>
+        <v>20</v>
+      </c>
+      <c r="G68" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H68" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I68">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>19</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>11</v>
+        <v>68</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="C69" s="6">
-        <v>152</v>
+        <v>821</v>
       </c>
       <c r="D69" s="6">
-        <v>141</v>
+        <v>821</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>30</v>
+        <v>134</v>
       </c>
       <c r="F69" s="8">
-        <v>4</v>
-      </c>
-      <c r="G69" s="27" t="s">
-        <v>31</v>
+        <v>20</v>
+      </c>
+      <c r="G69" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H69" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I69">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C70" s="6">
+        <v>825</v>
+      </c>
+      <c r="D70" s="6">
+        <v>825</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F70" s="8">
         <v>20</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C70" s="6">
-        <v>162</v>
-      </c>
-      <c r="D70" s="6">
-        <v>141</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F70" s="8">
-        <v>4</v>
-      </c>
-      <c r="G70" s="27" t="s">
-        <v>31</v>
+      <c r="G70" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H70" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I70">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C71" s="6">
+        <v>830</v>
+      </c>
+      <c r="D71" s="6">
+        <v>830</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F71" s="8">
         <v>21</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C71" s="6">
-        <v>164</v>
-      </c>
-      <c r="D71" s="6">
-        <v>141</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F71" s="8">
-        <v>4</v>
-      </c>
-      <c r="G71" s="27" t="s">
-        <v>31</v>
+      <c r="G71" s="29" t="s">
+        <v>921</v>
       </c>
       <c r="H71" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I71">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>26</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>9</v>
+        <v>71</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="C72" s="6">
-        <v>106</v>
+        <v>840</v>
       </c>
       <c r="D72" s="6">
-        <v>193</v>
+        <v>840</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="F72" s="8">
-        <v>6</v>
-      </c>
-      <c r="G72" s="9" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="G72" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H72" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I72">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>27</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>9</v>
+        <v>72</v>
+      </c>
+      <c r="B73" s="32" t="s">
+        <v>83</v>
       </c>
       <c r="C73" s="6">
-        <v>123</v>
+        <v>911</v>
       </c>
       <c r="D73" s="6">
-        <v>191</v>
+        <v>911</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="F73" s="8">
-        <v>6</v>
-      </c>
-      <c r="G73" s="9" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="G73" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H73" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I73">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>28</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>9</v>
+        <v>73</v>
+      </c>
+      <c r="B74" s="32" t="s">
+        <v>85</v>
       </c>
       <c r="C74" s="6">
-        <v>136</v>
+        <v>915</v>
       </c>
       <c r="D74" s="6">
-        <v>193</v>
+        <v>915</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="F74" s="8">
-        <v>6</v>
-      </c>
-      <c r="G74" s="9" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="G74" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H74" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I74">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>29</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>9</v>
+        <v>74</v>
+      </c>
+      <c r="B75" s="32" t="s">
+        <v>87</v>
       </c>
       <c r="C75" s="6">
-        <v>138</v>
+        <v>917</v>
       </c>
       <c r="D75" s="6">
-        <v>193</v>
+        <v>917</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>150</v>
+        <v>88</v>
       </c>
       <c r="F75" s="8">
-        <v>6</v>
-      </c>
-      <c r="G75" s="9" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="G75" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H75" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I75">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>30</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
+      </c>
+      <c r="B76" s="32" t="s">
+        <v>89</v>
       </c>
       <c r="C76" s="6">
-        <v>142</v>
+        <v>921</v>
       </c>
       <c r="D76" s="6">
-        <v>193</v>
+        <v>921</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="F76" s="8">
-        <v>6</v>
-      </c>
-      <c r="G76" s="9" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="G76" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H76" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I76">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>31</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>9</v>
+        <v>76</v>
+      </c>
+      <c r="B77" s="32" t="s">
+        <v>91</v>
       </c>
       <c r="C77" s="6">
-        <v>144</v>
+        <v>925</v>
       </c>
       <c r="D77" s="6">
-        <v>193</v>
+        <v>925</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="F77" s="8">
-        <v>6</v>
-      </c>
-      <c r="G77" s="9" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="G77" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="H77" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I77">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>32</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>9</v>
+        <v>77</v>
+      </c>
+      <c r="B78" s="31" t="s">
+        <v>97</v>
       </c>
       <c r="C78" s="6">
-        <v>177</v>
+        <v>944</v>
       </c>
       <c r="D78" s="6">
-        <v>191</v>
+        <v>944</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="F78" s="8">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="H78" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I78">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>33</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>9</v>
+        <v>78</v>
+      </c>
+      <c r="B79" s="31" t="s">
+        <v>97</v>
       </c>
       <c r="C79" s="6">
-        <v>2005</v>
-      </c>
-      <c r="D79" s="6">
-        <v>191</v>
+        <v>9311</v>
+      </c>
+      <c r="D79" s="11">
+        <v>931</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F79" s="8">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="H79" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I79">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>83</v>
-      </c>
-      <c r="B80" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="C80" s="37" t="s">
-        <v>166</v>
+        <v>79</v>
+      </c>
+      <c r="B80" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C80" s="6">
+        <v>9312</v>
       </c>
       <c r="D80" s="11">
-        <v>155</v>
-      </c>
-      <c r="E80" s="42" t="s">
-        <v>149</v>
+        <v>931</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="F80" s="8">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="H80" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I80">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="B81" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="C81" s="37">
-        <v>172</v>
-      </c>
-      <c r="D81" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="E81" s="32" t="s">
-        <v>169</v>
+        <v>100</v>
+      </c>
+      <c r="C81" s="6">
+        <v>945</v>
+      </c>
+      <c r="D81" s="6">
+        <v>932</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="F81" s="8">
-        <v>6</v>
-      </c>
-      <c r="G81" s="9" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="G81" s="27" t="s">
+        <v>94</v>
       </c>
       <c r="H81" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="I81">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>34</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>42</v>
+        <v>81</v>
+      </c>
+      <c r="B82" s="32" t="s">
+        <v>93</v>
       </c>
       <c r="C82" s="6">
-        <v>210</v>
-      </c>
-      <c r="D82" s="6">
-        <v>211</v>
+        <v>933</v>
+      </c>
+      <c r="D82" s="11">
+        <v>933</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="F82" s="8">
-        <v>7</v>
-      </c>
-      <c r="G82" s="9" t="s">
-        <v>44</v>
+        <v>23</v>
+      </c>
+      <c r="G82" s="27" t="s">
+        <v>94</v>
       </c>
       <c r="H82" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c r="I82">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>35</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>45</v>
+        <v>82</v>
+      </c>
+      <c r="B83" s="32" t="s">
+        <v>95</v>
       </c>
       <c r="C83" s="6">
-        <v>217</v>
+        <v>935</v>
       </c>
       <c r="D83" s="6">
-        <v>217</v>
+        <v>935</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="F83" s="13">
-        <v>7</v>
-      </c>
-      <c r="G83" s="9" t="s">
-        <v>44</v>
+        <v>23</v>
+      </c>
+      <c r="G83" s="27" t="s">
+        <v>94</v>
       </c>
       <c r="H83" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c r="I83">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>36</v>
-      </c>
-      <c r="B84" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="C84" s="39">
-        <v>2151</v>
+        <v>83</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>166</v>
       </c>
       <c r="D84" s="16">
-        <v>215</v>
-      </c>
-      <c r="E84" s="43" t="s">
-        <v>142</v>
+        <v>155</v>
+      </c>
+      <c r="E84" s="37" t="s">
+        <v>149</v>
       </c>
       <c r="F84" s="14">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G84" s="12" t="s">
-        <v>44</v>
+        <v>149</v>
       </c>
       <c r="H84" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="I84">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>37</v>
-      </c>
-      <c r="B85" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C85" s="39">
-        <v>2152</v>
+        <v>84</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C85" s="19" t="s">
+        <v>166</v>
       </c>
       <c r="D85" s="16">
-        <v>217</v>
-      </c>
-      <c r="E85" s="41" t="s">
-        <v>143</v>
+        <v>231</v>
+      </c>
+      <c r="E85" s="15" t="s">
+        <v>151</v>
       </c>
       <c r="F85" s="14">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="H85" t="s">
         <v>928</v>
@@ -5977,442 +5972,442 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>38</v>
-      </c>
-      <c r="B86" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C86" s="39">
-        <v>203</v>
-      </c>
-      <c r="D86" s="39">
-        <v>225</v>
-      </c>
-      <c r="E86" s="41" t="s">
-        <v>40</v>
+        <v>85</v>
+      </c>
+      <c r="B86" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="C86" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D86" s="16">
+        <v>411</v>
+      </c>
+      <c r="E86" s="34" t="s">
+        <v>152</v>
       </c>
       <c r="F86" s="14">
-        <v>8</v>
-      </c>
-      <c r="G86" s="12" t="s">
-        <v>41</v>
+        <v>18</v>
+      </c>
+      <c r="G86" s="41" t="s">
+        <v>924</v>
       </c>
       <c r="H86" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I86">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>39</v>
-      </c>
-      <c r="B87" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C87" s="38">
-        <v>221</v>
-      </c>
-      <c r="D87" s="6">
-        <v>221</v>
-      </c>
-      <c r="E87" s="40" t="s">
-        <v>46</v>
+        <v>86</v>
+      </c>
+      <c r="B87" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C87" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="D87" s="11">
+        <v>425</v>
+      </c>
+      <c r="E87" s="35" t="s">
+        <v>153</v>
       </c>
       <c r="F87" s="14">
-        <v>8</v>
-      </c>
-      <c r="G87" s="12" t="s">
-        <v>41</v>
+        <v>18</v>
+      </c>
+      <c r="G87" s="41" t="s">
+        <v>924</v>
       </c>
       <c r="H87" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I87">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>40</v>
-      </c>
-      <c r="B88" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C88" s="39">
-        <v>291</v>
-      </c>
-      <c r="D88" s="39">
-        <v>291</v>
-      </c>
-      <c r="E88" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="F88" s="14">
-        <v>9</v>
-      </c>
-      <c r="G88" s="12" t="s">
-        <v>120</v>
+        <v>87</v>
+      </c>
+      <c r="B88" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="C88" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D88" s="16">
+        <v>427</v>
+      </c>
+      <c r="E88" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="F88" s="39">
+        <v>18</v>
+      </c>
+      <c r="G88" s="41" t="s">
+        <v>924</v>
       </c>
       <c r="H88" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I88">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="B89" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="C89" s="39">
-        <v>960</v>
-      </c>
-      <c r="D89" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="C89" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="E89" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="F89" s="14">
-        <v>10</v>
-      </c>
-      <c r="G89" s="29" t="s">
-        <v>919</v>
+      <c r="D89" s="16">
+        <v>441</v>
+      </c>
+      <c r="E89" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="F89" s="39">
+        <v>19</v>
+      </c>
+      <c r="G89" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="H89" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I89">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>42</v>
-      </c>
-      <c r="B90" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="C90" s="39">
-        <v>310</v>
-      </c>
-      <c r="D90" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C90" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="E90" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="F90" s="14">
-        <v>10</v>
-      </c>
-      <c r="G90" s="29" t="s">
-        <v>919</v>
+      <c r="D90" s="16">
+        <v>451</v>
+      </c>
+      <c r="E90" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="F90" s="39">
+        <v>19</v>
+      </c>
+      <c r="G90" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="H90" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I90">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>43</v>
-      </c>
-      <c r="B91" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="C91" s="39">
-        <v>318</v>
-      </c>
-      <c r="D91" s="39">
-        <v>311</v>
-      </c>
-      <c r="E91" s="41" t="s">
-        <v>117</v>
+        <v>90</v>
+      </c>
+      <c r="B91" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="C91" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D91" s="16">
+        <v>461</v>
+      </c>
+      <c r="E91" s="33" t="s">
+        <v>156</v>
       </c>
       <c r="F91" s="14">
-        <v>10</v>
-      </c>
-      <c r="G91" s="46" t="s">
-        <v>919</v>
+        <v>18</v>
+      </c>
+      <c r="G91" s="41" t="s">
+        <v>924</v>
       </c>
       <c r="H91" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I91">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>44</v>
-      </c>
-      <c r="B92" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C92" s="39">
-        <v>200</v>
-      </c>
-      <c r="D92" s="39">
-        <v>331</v>
-      </c>
-      <c r="E92" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="F92" s="14">
-        <v>11</v>
-      </c>
-      <c r="G92" s="9" t="s">
-        <v>146</v>
+        <v>91</v>
+      </c>
+      <c r="B92" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="C92" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D92" s="16">
+        <v>471</v>
+      </c>
+      <c r="E92" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="F92" s="39">
+        <v>19</v>
+      </c>
+      <c r="G92" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="H92" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I92">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>45</v>
-      </c>
-      <c r="B93" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C93" s="39">
-        <v>315</v>
-      </c>
-      <c r="D93" s="39">
-        <v>315</v>
-      </c>
-      <c r="E93" s="41" t="s">
-        <v>125</v>
-      </c>
-      <c r="F93" s="13">
-        <v>11</v>
-      </c>
-      <c r="G93" s="9" t="s">
-        <v>146</v>
+        <v>92</v>
+      </c>
+      <c r="B93" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="C93" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D93" s="16">
+        <v>473</v>
+      </c>
+      <c r="E93" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="F93" s="40">
+        <v>19</v>
+      </c>
+      <c r="G93" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="H93" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I93">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>46</v>
-      </c>
-      <c r="B94" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C94" s="39">
-        <v>317</v>
-      </c>
-      <c r="D94" s="39">
-        <v>317</v>
-      </c>
-      <c r="E94" s="41" t="s">
-        <v>126</v>
-      </c>
-      <c r="F94" s="14">
-        <v>11</v>
-      </c>
-      <c r="G94" s="9" t="s">
-        <v>146</v>
+        <v>93</v>
+      </c>
+      <c r="B94" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="C94" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D94" s="16">
+        <v>475</v>
+      </c>
+      <c r="E94" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="F94" s="39">
+        <v>19</v>
+      </c>
+      <c r="G94" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="H94" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I94">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>47</v>
-      </c>
-      <c r="B95" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C95" s="39">
-        <v>319</v>
-      </c>
-      <c r="D95" s="39">
-        <v>321</v>
-      </c>
-      <c r="E95" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="F95" s="14">
-        <v>10</v>
-      </c>
-      <c r="G95" s="29" t="s">
-        <v>919</v>
+        <v>94</v>
+      </c>
+      <c r="B95" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C95" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D95" s="16">
+        <v>477</v>
+      </c>
+      <c r="E95" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="F95" s="39">
+        <v>19</v>
+      </c>
+      <c r="G95" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="H95" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I95">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>48</v>
-      </c>
-      <c r="B96" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C96" s="39">
-        <v>2008</v>
+        <v>95</v>
+      </c>
+      <c r="B96" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="C96" s="19" t="s">
+        <v>166</v>
       </c>
       <c r="D96" s="16">
-        <v>321</v>
-      </c>
-      <c r="E96" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="F96" s="14">
-        <v>10</v>
-      </c>
-      <c r="G96" s="29" t="s">
-        <v>919</v>
+        <v>479</v>
+      </c>
+      <c r="E96" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="F96" s="39">
+        <v>19</v>
+      </c>
+      <c r="G96" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="H96" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I96">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>49</v>
-      </c>
-      <c r="B97" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="C97" s="39">
-        <v>332</v>
-      </c>
-      <c r="D97" s="39">
-        <v>331</v>
-      </c>
-      <c r="E97" s="41" t="s">
-        <v>51</v>
+        <v>96</v>
+      </c>
+      <c r="B97" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="C97" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D97" s="16">
+        <v>570</v>
+      </c>
+      <c r="E97" s="33" t="s">
+        <v>159</v>
       </c>
       <c r="F97" s="13">
-        <v>12</v>
-      </c>
-      <c r="G97" s="9" t="s">
-        <v>51</v>
+        <v>21</v>
+      </c>
+      <c r="G97" s="29" t="s">
+        <v>921</v>
       </c>
       <c r="H97" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c r="I97">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="B98" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C98" s="39">
-        <v>341</v>
-      </c>
-      <c r="D98" s="39">
-        <v>341</v>
-      </c>
-      <c r="E98" s="41" t="s">
-        <v>53</v>
+        <v>160</v>
+      </c>
+      <c r="C98" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D98" s="16">
+        <v>611</v>
+      </c>
+      <c r="E98" s="33" t="s">
+        <v>160</v>
       </c>
       <c r="F98" s="13">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G98" s="29" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="H98" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c r="I98">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="B99" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C99" s="39">
-        <v>345</v>
-      </c>
-      <c r="D99" s="39">
-        <v>345</v>
-      </c>
-      <c r="E99" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="F99" s="13">
-        <v>13</v>
-      </c>
-      <c r="G99" s="29" t="s">
-        <v>922</v>
+        <v>165</v>
+      </c>
+      <c r="C99" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D99" s="16">
+        <v>465</v>
+      </c>
+      <c r="E99" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="F99" s="40">
+        <v>19</v>
+      </c>
+      <c r="G99" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="H99" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I99">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>84</v>
-      </c>
-      <c r="B100" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C100" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B100" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="C100" s="19">
+        <v>172</v>
+      </c>
+      <c r="D100" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="D100" s="16">
-        <v>231</v>
-      </c>
-      <c r="E100" s="15" t="s">
-        <v>151</v>
+      <c r="E100" s="33" t="s">
+        <v>169</v>
       </c>
       <c r="F100" s="8">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="H100" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="I100">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:I100">
-    <sortCondition ref="H1"/>
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
he terminado de reclasificar el codigo 16, he añadido la lista definitiva en el excel, por lo que ahora hay 16 Herbaceo secano y 18 Herbaceo regadio
</commit_message>
<xml_diff>
--- a/Correspondencias_SIOSE - modificada (v5).xlsx
+++ b/Correspondencias_SIOSE - modificada (v5).xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Correspondencia inicial" sheetId="2" r:id="rId2"/>
+    <sheet name="Lista definitiva usos" sheetId="3" r:id="rId2"/>
+    <sheet name="Correspondencia inicial" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2781" uniqueCount="933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2837" uniqueCount="935">
   <si>
     <t>SIOSE</t>
   </si>
@@ -2837,6 +2838,12 @@
   </si>
   <si>
     <t>Cobertura vegetal y suelos</t>
+  </si>
+  <si>
+    <t>Herbaceo secano</t>
+  </si>
+  <si>
+    <t>Herbaceo regadio</t>
   </si>
 </sst>
 </file>
@@ -3104,7 +3111,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
@@ -3200,6 +3207,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3492,7 +3502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="F63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:I100"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6414,6 +6426,406 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>930</v>
+      </c>
+      <c r="D1" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>926</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>926</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>926</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>926</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>926</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>918</v>
+      </c>
+      <c r="C7" t="s">
+        <v>929</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>926</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>928</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>928</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" t="s">
+        <v>928</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>919</v>
+      </c>
+      <c r="C12" t="s">
+        <v>928</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" t="s">
+        <v>928</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>928</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>13</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>922</v>
+      </c>
+      <c r="C15" t="s">
+        <v>928</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>927</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
+        <v>927</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>16</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>933</v>
+      </c>
+      <c r="C18" t="s">
+        <v>927</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>17</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>923</v>
+      </c>
+      <c r="C19" t="s">
+        <v>927</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>18</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>934</v>
+      </c>
+      <c r="C20" t="s">
+        <v>927</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>19</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>927</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="42">
+        <v>19</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" t="s">
+        <v>927</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>20</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>920</v>
+      </c>
+      <c r="C23" t="s">
+        <v>932</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>21</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>921</v>
+      </c>
+      <c r="C24" t="s">
+        <v>932</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>22</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" t="s">
+        <v>932</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>23</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" t="s">
+        <v>932</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>24</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" t="s">
+        <v>926</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D27">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>

</xml_diff>

<commit_message>
he cambiado de categoria general Mineria y residuos por Urbano e infraestructuras, debido al pequeño tamaño de poligonos de este tipo. Aun queda cambiarlo en las capas de QGIS
</commit_message>
<xml_diff>
--- a/Correspondencias_SIOSE - modificada (v5).xlsx
+++ b/Correspondencias_SIOSE - modificada (v5).xlsx
@@ -6430,7 +6430,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D6" sqref="D6:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6531,10 +6531,10 @@
         <v>918</v>
       </c>
       <c r="C7" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
he añadido la columna de valores de presion o impacto a los usos del suelo
</commit_message>
<xml_diff>
--- a/Correspondencias_SIOSE - modificada (v5).xlsx
+++ b/Correspondencias_SIOSE - modificada (v5).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\MASTER\TFM\rTFM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\TFM\rTFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2837" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2838" uniqueCount="936">
   <si>
     <t>SIOSE</t>
   </si>
@@ -2844,6 +2844,9 @@
   </si>
   <si>
     <t>Herbaceo regadio</t>
+  </si>
+  <si>
+    <t>COD_PRESION</t>
   </si>
 </sst>
 </file>
@@ -6427,10 +6430,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6439,7 +6442,7 @@
     <col min="2" max="2" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -6452,8 +6455,11 @@
       <c r="D1" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>0</v>
       </c>
@@ -6466,8 +6472,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -6480,8 +6489,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -6494,8 +6506,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -6508,8 +6523,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -6522,8 +6540,11 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -6536,8 +6557,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -6550,8 +6574,11 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -6564,8 +6591,11 @@
       <c r="D9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -6578,8 +6608,11 @@
       <c r="D10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -6592,8 +6625,11 @@
       <c r="D11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -6606,8 +6642,11 @@
       <c r="D12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -6620,8 +6659,11 @@
       <c r="D13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -6634,8 +6676,11 @@
       <c r="D14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -6648,8 +6693,11 @@
       <c r="D15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -6662,8 +6710,11 @@
       <c r="D16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -6676,8 +6727,11 @@
       <c r="D17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>16</v>
       </c>
@@ -6690,8 +6744,11 @@
       <c r="D18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>17</v>
       </c>
@@ -6702,10 +6759,13 @@
         <v>927</v>
       </c>
       <c r="D19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>18</v>
       </c>
@@ -6718,8 +6778,11 @@
       <c r="D20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>19</v>
       </c>
@@ -6732,8 +6795,11 @@
       <c r="D21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="42">
         <v>19</v>
       </c>
@@ -6746,8 +6812,11 @@
       <c r="D22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>20</v>
       </c>
@@ -6760,8 +6829,11 @@
       <c r="D23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>21</v>
       </c>
@@ -6774,8 +6846,11 @@
       <c r="D24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>22</v>
       </c>
@@ -6788,8 +6863,11 @@
       <c r="D25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>23</v>
       </c>
@@ -6802,8 +6880,11 @@
       <c r="D26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>24</v>
       </c>
@@ -6815,12 +6896,27 @@
       </c>
       <c r="D27">
         <v>1</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:D27">
     <sortCondition ref="A2"/>
   </sortState>
+  <conditionalFormatting sqref="E2:E27">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
he unido la columna de Presion a las capas de usos del suelo y he añadido una nota con la tutoria de hoy 18 de septiembre
</commit_message>
<xml_diff>
--- a/Correspondencias_SIOSE - modificada (v5).xlsx
+++ b/Correspondencias_SIOSE - modificada (v5).xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2838" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2838" uniqueCount="937">
   <si>
     <t>SIOSE</t>
   </si>
@@ -2847,6 +2847,9 @@
   </si>
   <si>
     <t>COD_PRESION</t>
+  </si>
+  <si>
+    <t>Agrario invernaderos</t>
   </si>
 </sst>
 </file>
@@ -6432,8 +6435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6756,7 +6759,7 @@
         <v>923</v>
       </c>
       <c r="C19" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="D19">
         <v>2</v>

</xml_diff>

<commit_message>
he renombrado los scripts de R y he administrado los archivos de GEE, ya que estoy exportando ahora los archivos de NDWI
</commit_message>
<xml_diff>
--- a/Correspondencias_SIOSE - modificada (v5).xlsx
+++ b/Correspondencias_SIOSE - modificada (v5).xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2838" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2834" uniqueCount="935">
   <si>
     <t>SIOSE</t>
   </si>
@@ -2838,12 +2838,6 @@
   </si>
   <si>
     <t>Cobertura vegetal y suelos</t>
-  </si>
-  <si>
-    <t>Herbaceo secano</t>
-  </si>
-  <si>
-    <t>Herbaceo regadio</t>
   </si>
   <si>
     <t>COD_PRESION</t>
@@ -3117,7 +3111,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
@@ -3213,9 +3207,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3508,7 +3499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView topLeftCell="F63" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D79" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:I100"/>
     </sheetView>
   </sheetViews>
@@ -6433,10 +6424,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6459,7 +6450,7 @@
         <v>931</v>
       </c>
       <c r="E1" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6736,44 +6727,44 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <v>16</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>933</v>
+        <v>17</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>923</v>
       </c>
       <c r="C18" t="s">
-        <v>927</v>
+        <v>934</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C19" t="s">
-        <v>936</v>
+        <v>927</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <v>18</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>934</v>
+        <v>19</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C20" t="s">
         <v>927</v>
@@ -6787,44 +6778,44 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <v>19</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>920</v>
       </c>
       <c r="C21" t="s">
-        <v>927</v>
+        <v>932</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="42">
-        <v>19</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>168</v>
+      <c r="A22" s="8">
+        <v>21</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>921</v>
       </c>
       <c r="C22" t="s">
-        <v>927</v>
+        <v>932</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E22">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <v>20</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>920</v>
+        <v>22</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="C23" t="s">
         <v>932</v>
@@ -6838,10 +6829,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <v>21</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>921</v>
+        <v>23</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>94</v>
       </c>
       <c r="C24" t="s">
         <v>932</v>
@@ -6850,57 +6841,23 @@
         <v>5</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="C25" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
-        <v>23</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" t="s">
-        <v>932</v>
-      </c>
-      <c r="D26">
-        <v>5</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
-        <v>24</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C27" t="s">
-        <v>926</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
         <v>4</v>
       </c>
     </row>
@@ -6908,8 +6865,8 @@
   <sortState ref="A2:D27">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="E2:E27">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="E2:E25">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6921,6 +6878,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
he hecho una tabla de los cambios de usos del suelo por humedal y he avanzado en el calculo de porcentaje de usos del suelo tanto para MUCVA como para SIOSE
</commit_message>
<xml_diff>
--- a/Correspondencias_SIOSE - modificada (v5).xlsx
+++ b/Correspondencias_SIOSE - modificada (v5).xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2834" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2834" uniqueCount="936">
   <si>
     <t>SIOSE</t>
   </si>
@@ -2844,6 +2844,9 @@
   </si>
   <si>
     <t>Agrario invernaderos</t>
+  </si>
+  <si>
+    <t>Areas agrarias heterogeneas</t>
   </si>
 </sst>
 </file>
@@ -6426,8 +6429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6764,7 +6767,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>12</v>
+        <v>935</v>
       </c>
       <c r="C20" t="s">
         <v>927</v>

</xml_diff>